<commit_message>
Deep learning Convolutional Neural Network
</commit_message>
<xml_diff>
--- a/Collaborative Filtering Smaple.xlsx
+++ b/Collaborative Filtering Smaple.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Eigen Values Vectors" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Person1">Sheet1!$P$28:$V$28</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="28">
   <si>
     <t>Person1</t>
   </si>
@@ -99,18 +100,48 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF020202"/>
+      <name val="Inherit"/>
     </font>
   </fonts>
   <fills count="2">
@@ -121,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -209,11 +240,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFEBEBEB"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFEBEBEB"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFEBEBEB"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFEBEBEB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -225,6 +271,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,6 +289,913 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Eigen Values Vectors'!$L$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Eigen Values Vectors'!$K$35:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Eigen Values Vectors'!$L$35:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2EC-403D-AB49-5E5CD3E4B7F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2086592560"/>
+        <c:axId val="2086592976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2086592560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2086592976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2086592976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2086592560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -507,13 +1463,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1">
       <c r="H1" t="s">
         <v>12</v>
       </c>
@@ -557,12 +1513,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23">
       <c r="A2">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -581,40 +1537,40 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1">
-        <f>IF(H2&lt;&gt;"",H2,(AVERAGE($H2:$N2)+AVERAGE(H$2:H$13)) /2)</f>
+        <f t="shared" ref="Q2:W2" si="0">IF(H2&lt;&gt;"",H2,(AVERAGE($H2:$N2)+AVERAGE(H$2:H$13)) /2)</f>
         <v>1</v>
       </c>
       <c r="R2" s="2">
-        <f>IF(I2&lt;&gt;"",I2,(AVERAGE($H2:$N2)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>2.6</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="S2" s="2">
-        <f>IF(J2&lt;&gt;"",J2,(AVERAGE($H2:$N2)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="T2" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="U2" s="2">
+        <f t="shared" si="0"/>
+        <v>2.625</v>
+      </c>
+      <c r="V2" s="2">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="T2" s="2">
-        <f>IF(K2&lt;&gt;"",K2,(AVERAGE($H2:$N2)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>1.7</v>
-      </c>
-      <c r="U2" s="2">
-        <f>IF(L2&lt;&gt;"",L2,(AVERAGE($H2:$N2)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>2.625</v>
-      </c>
-      <c r="V2" s="2">
-        <f>IF(M2&lt;&gt;"",M2,(AVERAGE($H2:$N2)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>1.5</v>
-      </c>
       <c r="W2" s="3">
-        <f>IF(N2&lt;&gt;"",N2,(AVERAGE($H2:$N2)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
@@ -633,40 +1589,40 @@
         <v>1</v>
       </c>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q13" si="0">IF(H3&lt;&gt;"",H3,(AVERAGE($H3:$N3)+AVERAGE(H$2:H$13)) /2)</f>
+        <f t="shared" ref="Q3:Q13" si="1">IF(H3&lt;&gt;"",H3,(AVERAGE($H3:$N3)+AVERAGE(H$2:H$13)) /2)</f>
         <v>1.3333333333333335</v>
       </c>
       <c r="R3" s="5">
-        <f>IF(I3&lt;&gt;"",I3,(AVERAGE($H3:$N3)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>2.6</v>
+        <f t="shared" ref="R3:R13" si="2">IF(I3&lt;&gt;"",I3,(AVERAGE($H3:$N3)+AVERAGE(I$2:I$13)) /2)</f>
+        <v>2</v>
       </c>
       <c r="S3" s="5">
-        <f>IF(J3&lt;&gt;"",J3,(AVERAGE($H3:$N3)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" ref="S3:S13" si="3">IF(J3&lt;&gt;"",J3,(AVERAGE($H3:$N3)+AVERAGE(J$2:J$13)) /2)</f>
+        <v>1.6</v>
+      </c>
+      <c r="T3" s="5">
+        <f t="shared" ref="T3:T13" si="4">IF(K3&lt;&gt;"",K3,(AVERAGE($H3:$N3)+AVERAGE(K$2:K$13)) /2)</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="5">
+        <f t="shared" ref="U3:U13" si="5">IF(L3&lt;&gt;"",L3,(AVERAGE($H3:$N3)+AVERAGE(L$2:L$13)) /2)</f>
+        <v>2.625</v>
+      </c>
+      <c r="V3" s="5">
+        <f t="shared" ref="V3:V13" si="6">IF(M3&lt;&gt;"",M3,(AVERAGE($H3:$N3)+AVERAGE(M$2:M$13)) /2)</f>
         <v>1.5</v>
       </c>
-      <c r="T3" s="5">
-        <f>IF(K3&lt;&gt;"",K3,(AVERAGE($H3:$N3)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>1</v>
-      </c>
-      <c r="U3" s="5">
-        <f>IF(L3&lt;&gt;"",L3,(AVERAGE($H3:$N3)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>2.625</v>
-      </c>
-      <c r="V3" s="5">
-        <f>IF(M3&lt;&gt;"",M3,(AVERAGE($H3:$N3)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>1.5</v>
-      </c>
       <c r="W3" s="6">
-        <f>IF(N3&lt;&gt;"",N3,(AVERAGE($H3:$N3)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" ref="W3:W13" si="7">IF(N3&lt;&gt;"",N3,(AVERAGE($H3:$N3)+AVERAGE(N$2:N$13)) /2)</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
@@ -685,40 +1641,40 @@
         <v>2</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="R4" s="5">
-        <f>IF(I4&lt;&gt;"",I4,(AVERAGE($H4:$N4)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="S4" s="5">
-        <f>IF(J4&lt;&gt;"",J4,(AVERAGE($H4:$N4)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="3"/>
+        <v>3.6</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="4"/>
+        <v>3.7</v>
+      </c>
+      <c r="U4" s="5">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="V4" s="5">
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
-      <c r="T4" s="5">
-        <f>IF(K4&lt;&gt;"",K4,(AVERAGE($H4:$N4)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>3.7</v>
-      </c>
-      <c r="U4" s="5">
-        <f>IF(L4&lt;&gt;"",L4,(AVERAGE($H4:$N4)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>5</v>
-      </c>
-      <c r="V4" s="5">
-        <f>IF(M4&lt;&gt;"",M4,(AVERAGE($H4:$N4)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>3.5</v>
-      </c>
       <c r="W4" s="6">
-        <f>IF(N4&lt;&gt;"",N4,(AVERAGE($H4:$N4)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -727,10 +1683,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K5" s="5">
         <v>4</v>
@@ -743,35 +1699,41 @@
         <v>3</v>
       </c>
       <c r="Q5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="R5" s="5">
-        <f>IF(I5&lt;&gt;"",I5,(AVERAGE($H5:$N5)+AVERAGE(I$2:I$13)) /2)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="5">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T5" s="5">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="S5" s="5">
-        <f>IF(J5&lt;&gt;"",J5,(AVERAGE($H5:$N5)+AVERAGE(J$2:J$13)) /2)</f>
-        <v>1</v>
-      </c>
-      <c r="T5" s="5">
-        <f>IF(K5&lt;&gt;"",K5,(AVERAGE($H5:$N5)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>4</v>
-      </c>
       <c r="U5" s="5">
-        <f>IF(L5&lt;&gt;"",L5,(AVERAGE($H5:$N5)+AVERAGE(L$2:L$13)) /2)</f>
+        <f t="shared" si="5"/>
         <v>3.75</v>
       </c>
       <c r="V5" s="5">
-        <f>IF(M5&lt;&gt;"",M5,(AVERAGE($H5:$N5)+AVERAGE(M$2:M$13)) /2)</f>
+        <f t="shared" si="6"/>
         <v>2.625</v>
       </c>
       <c r="W5" s="6">
-        <f>IF(N5&lt;&gt;"",N5,(AVERAGE($H5:$N5)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>4.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
@@ -779,10 +1741,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K6" s="10">
         <v>0</v>
@@ -797,44 +1759,50 @@
         <v>4</v>
       </c>
       <c r="Q6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R6" s="5">
-        <f>IF(I6&lt;&gt;"",I6,(AVERAGE($H6:$N6)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="S6" s="5">
-        <f>IF(J6&lt;&gt;"",J6,(AVERAGE($H6:$N6)+AVERAGE(J$2:J$13)) /2)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="T6" s="5">
-        <f>IF(K6&lt;&gt;"",K6,(AVERAGE($H6:$N6)+AVERAGE(K$2:K$13)) /2)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="U6" s="5">
-        <f>IF(L6&lt;&gt;"",L6,(AVERAGE($H6:$N6)+AVERAGE(L$2:L$13)) /2)</f>
+        <f t="shared" si="5"/>
         <v>2.7250000000000001</v>
       </c>
       <c r="V6" s="5">
-        <f>IF(M6&lt;&gt;"",M6,(AVERAGE($H6:$N6)+AVERAGE(M$2:M$13)) /2)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="W6" s="6">
-        <f>IF(N6&lt;&gt;"",N6,(AVERAGE($H6:$N6)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
       <c r="G7" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J7" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -845,35 +1813,41 @@
         <v>5</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="0"/>
-        <v>2.8333333333333335</v>
+        <f t="shared" si="1"/>
+        <v>2.0833333333333335</v>
       </c>
       <c r="R7" s="5">
-        <f>IF(I7&lt;&gt;"",I7,(AVERAGE($H7:$N7)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="S7" s="5">
-        <f>IF(J7&lt;&gt;"",J7,(AVERAGE($H7:$N7)+AVERAGE(J$2:J$13)) /2)</f>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="T7" s="5">
-        <f>IF(K7&lt;&gt;"",K7,(AVERAGE($H7:$N7)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>3.2</v>
+        <f t="shared" si="4"/>
+        <v>2.4500000000000002</v>
       </c>
       <c r="U7" s="5">
-        <f>IF(L7&lt;&gt;"",L7,(AVERAGE($H7:$N7)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>4.125</v>
+        <f t="shared" si="5"/>
+        <v>3.375</v>
       </c>
       <c r="V7" s="5">
-        <f>IF(M7&lt;&gt;"",M7,(AVERAGE($H7:$N7)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>2.25</v>
       </c>
       <c r="W7" s="6">
-        <f>IF(N7&lt;&gt;"",N7,(AVERAGE($H7:$N7)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
       <c r="G8" t="s">
         <v>6</v>
       </c>
@@ -882,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="5">
         <v>4</v>
@@ -890,42 +1864,48 @@
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O8" s="5"/>
       <c r="P8" t="s">
         <v>6</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="0"/>
-        <v>2.8333333333333335</v>
+        <f t="shared" si="1"/>
+        <v>1.9583333333333335</v>
       </c>
       <c r="R8" s="5">
-        <f>IF(I8&lt;&gt;"",I8,(AVERAGE($H8:$N8)+AVERAGE(I$2:I$13)) /2)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="S8" s="5">
-        <f>IF(J8&lt;&gt;"",J8,(AVERAGE($H8:$N8)+AVERAGE(J$2:J$13)) /2)</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="T8" s="5">
-        <f>IF(K8&lt;&gt;"",K8,(AVERAGE($H8:$N8)+AVERAGE(K$2:K$13)) /2)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="U8" s="5">
-        <f>IF(L8&lt;&gt;"",L8,(AVERAGE($H8:$N8)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>4.125</v>
+        <f t="shared" si="5"/>
+        <v>3.25</v>
       </c>
       <c r="V8" s="5">
-        <f>IF(M8&lt;&gt;"",M8,(AVERAGE($H8:$N8)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>2.125</v>
       </c>
       <c r="W8" s="6">
-        <f>IF(N8&lt;&gt;"",N8,(AVERAGE($H8:$N8)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
@@ -949,35 +1929,35 @@
         <v>7</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.8333333333333335</v>
       </c>
       <c r="R9" s="5">
-        <f>IF(I9&lt;&gt;"",I9,(AVERAGE($H9:$N9)+AVERAGE(I$2:I$13)) /2)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="S9" s="5">
-        <f>IF(J9&lt;&gt;"",J9,(AVERAGE($H9:$N9)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="T9" s="5">
-        <f>IF(K9&lt;&gt;"",K9,(AVERAGE($H9:$N9)+AVERAGE(K$2:K$13)) /2)</f>
+        <f t="shared" si="4"/>
         <v>3.2</v>
       </c>
       <c r="U9" s="5">
-        <f>IF(L9&lt;&gt;"",L9,(AVERAGE($H9:$N9)+AVERAGE(L$2:L$13)) /2)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="V9" s="5">
-        <f>IF(M9&lt;&gt;"",M9,(AVERAGE($H9:$N9)+AVERAGE(M$2:M$13)) /2)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="W9" s="6">
-        <f>IF(N9&lt;&gt;"",N9,(AVERAGE($H9:$N9)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="G10" t="s">
         <v>8</v>
       </c>
@@ -995,35 +1975,35 @@
         <v>8</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="R10" s="5">
-        <f>IF(I10&lt;&gt;"",I10,(AVERAGE($H10:$N10)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>3.6</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="S10" s="5">
-        <f>IF(J10&lt;&gt;"",J10,(AVERAGE($H10:$N10)+AVERAGE(J$2:J$13)) /2)</f>
-        <v>2.5</v>
+        <f t="shared" si="3"/>
+        <v>2.6</v>
       </c>
       <c r="T10" s="5">
-        <f>IF(K10&lt;&gt;"",K10,(AVERAGE($H10:$N10)+AVERAGE(K$2:K$13)) /2)</f>
+        <f t="shared" si="4"/>
         <v>2.7</v>
       </c>
       <c r="U10" s="5">
-        <f>IF(L10&lt;&gt;"",L10,(AVERAGE($H10:$N10)+AVERAGE(L$2:L$13)) /2)</f>
+        <f t="shared" si="5"/>
         <v>3.625</v>
       </c>
       <c r="V10" s="5">
-        <f>IF(M10&lt;&gt;"",M10,(AVERAGE($H10:$N10)+AVERAGE(M$2:M$13)) /2)</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="W10" s="6">
-        <f>IF(N10&lt;&gt;"",N10,(AVERAGE($H10:$N10)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="G11" t="s">
         <v>9</v>
       </c>
@@ -1041,35 +2021,35 @@
         <v>9</v>
       </c>
       <c r="Q11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.3333333333333335</v>
       </c>
       <c r="R11" s="5">
-        <f>IF(I11&lt;&gt;"",I11,(AVERAGE($H11:$N11)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>3.6</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="S11" s="5">
-        <f>IF(J11&lt;&gt;"",J11,(AVERAGE($H11:$N11)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="3"/>
+        <v>2.6</v>
+      </c>
+      <c r="T11" s="5">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="U11" s="5">
+        <f t="shared" si="5"/>
+        <v>3.625</v>
+      </c>
+      <c r="V11" s="5">
+        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
-      <c r="T11" s="5">
-        <f>IF(K11&lt;&gt;"",K11,(AVERAGE($H11:$N11)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>3</v>
-      </c>
-      <c r="U11" s="5">
-        <f>IF(L11&lt;&gt;"",L11,(AVERAGE($H11:$N11)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>3.625</v>
-      </c>
-      <c r="V11" s="5">
-        <f>IF(M11&lt;&gt;"",M11,(AVERAGE($H11:$N11)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>2.5</v>
-      </c>
       <c r="W11" s="6">
-        <f>IF(N11&lt;&gt;"",N11,(AVERAGE($H11:$N11)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="G12" t="s">
         <v>10</v>
       </c>
@@ -1087,35 +2067,35 @@
         <v>10</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8333333333333335</v>
       </c>
       <c r="R12" s="5">
-        <f>IF(I12&lt;&gt;"",I12,(AVERAGE($H12:$N12)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>3.1</v>
+        <f t="shared" si="2"/>
+        <v>2.5</v>
       </c>
       <c r="S12" s="5">
-        <f>IF(J12&lt;&gt;"",J12,(AVERAGE($H12:$N12)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
+      <c r="T12" s="5">
+        <f t="shared" si="4"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U12" s="5">
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="T12" s="5">
-        <f>IF(K12&lt;&gt;"",K12,(AVERAGE($H12:$N12)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="U12" s="5">
-        <f>IF(L12&lt;&gt;"",L12,(AVERAGE($H12:$N12)+AVERAGE(L$2:L$13)) /2)</f>
+      <c r="V12" s="5">
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="V12" s="5">
-        <f>IF(M12&lt;&gt;"",M12,(AVERAGE($H12:$N12)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>2</v>
-      </c>
       <c r="W12" s="6">
-        <f>IF(N12&lt;&gt;"",N12,(AVERAGE($H12:$N12)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" thickBot="1">
       <c r="G13" t="s">
         <v>11</v>
       </c>
@@ -1133,46 +2113,46 @@
         <v>11</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="R13" s="8">
-        <f>IF(I13&lt;&gt;"",I13,(AVERAGE($H13:$N13)+AVERAGE(I$2:I$13)) /2)</f>
-        <v>4.5999999999999996</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="S13" s="8">
-        <f>IF(J13&lt;&gt;"",J13,(AVERAGE($H13:$N13)+AVERAGE(J$2:J$13)) /2)</f>
+        <f t="shared" si="3"/>
+        <v>3.6</v>
+      </c>
+      <c r="T13" s="8">
+        <f t="shared" si="4"/>
+        <v>3.7</v>
+      </c>
+      <c r="U13" s="8">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="V13" s="8">
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
-      <c r="T13" s="8">
-        <f>IF(K13&lt;&gt;"",K13,(AVERAGE($H13:$N13)+AVERAGE(K$2:K$13)) /2)</f>
-        <v>3.7</v>
-      </c>
-      <c r="U13" s="8">
-        <f>IF(L13&lt;&gt;"",L13,(AVERAGE($H13:$N13)+AVERAGE(L$2:L$13)) /2)</f>
-        <v>5</v>
-      </c>
-      <c r="V13" s="8">
-        <f>IF(M13&lt;&gt;"",M13,(AVERAGE($H13:$N13)+AVERAGE(M$2:M$13)) /2)</f>
-        <v>3.5</v>
-      </c>
       <c r="W13" s="9">
-        <f>IF(N13&lt;&gt;"",N13,(AVERAGE($H13:$N13)+AVERAGE(N$2:N$13)) /2)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="10:38" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="18" spans="10:38">
       <c r="V18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:38">
       <c r="J20">
         <f>SUMPRODUCT(A$2:A$9,B2:B9)/(SQRT(SUMSQ(B2:B9))*SQRT(SUMSQ($A$2:$A$9)))</f>
-        <v>-0.24207264988525407</v>
-      </c>
-    </row>
-    <row r="22" spans="10:38" x14ac:dyDescent="0.25">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="22" spans="10:38">
       <c r="AA22" t="s">
         <v>0</v>
       </c>
@@ -1210,7 +2190,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="10:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:38" ht="15.75" thickBot="1">
       <c r="P27" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +2213,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="10:38" ht="17.25" thickBot="1">
       <c r="L28">
         <f ca="1">SUM(INDIRECT(O28))</f>
         <v>1</v>
@@ -1250,8 +2230,9 @@
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="3"/>
-    </row>
-    <row r="29" spans="10:38" x14ac:dyDescent="0.25">
+      <c r="W28" s="11"/>
+    </row>
+    <row r="29" spans="10:38">
       <c r="L29">
         <f ca="1">SUM(INDIRECT(O29))</f>
         <v>1</v>
@@ -1269,7 +2250,7 @@
       <c r="U29" s="5"/>
       <c r="V29" s="6"/>
     </row>
-    <row r="30" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="10:38">
       <c r="L30">
         <f ca="1">SUM(INDIRECT(O30))</f>
         <v>7</v>
@@ -1289,7 +2270,7 @@
       <c r="U30" s="5"/>
       <c r="V30" s="6"/>
     </row>
-    <row r="31" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="10:38">
       <c r="O31" t="s">
         <v>3</v>
       </c>
@@ -1309,7 +2290,7 @@
       <c r="U31" s="5"/>
       <c r="V31" s="6"/>
     </row>
-    <row r="32" spans="10:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="10:38">
       <c r="O32" t="s">
         <v>4</v>
       </c>
@@ -1331,7 +2312,15 @@
       </c>
       <c r="V32" s="6"/>
     </row>
-    <row r="33" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:22">
+      <c r="L33" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(M33),INDIRECT(L34)/(SQRT(SUMSQ(M33))*SQRT(SUMSQ(L34))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M33" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(N33),INDIRECT(M34)/(SQRT(SUMSQ(N33))*SQRT(SUMSQ(M34))))</f>
+        <v>#REF!</v>
+      </c>
       <c r="O33" t="s">
         <v>5</v>
       </c>
@@ -1345,7 +2334,27 @@
       <c r="U33" s="5"/>
       <c r="V33" s="6"/>
     </row>
-    <row r="34" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:22">
+      <c r="J34" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(K34),INDIRECT(J35)/(SQRT(SUMSQ(K34))*SQRT(SUMSQ(J35))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K34" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(L34),INDIRECT(K35)/(SQRT(SUMSQ(L34))*SQRT(SUMSQ(K35))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L34" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(M34),INDIRECT(L35)/(SQRT(SUMSQ(M34))*SQRT(SUMSQ(L35))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M34" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(N34),INDIRECT(M35)/(SQRT(SUMSQ(N34))*SQRT(SUMSQ(M35))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N34" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(O34),INDIRECT(N35)/(SQRT(SUMSQ(O34))*SQRT(SUMSQ(N35))))</f>
+        <v>#REF!</v>
+      </c>
       <c r="O34" t="s">
         <v>6</v>
       </c>
@@ -1361,7 +2370,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:22">
+      <c r="J35" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(K35),INDIRECT(J36)/(SQRT(SUMSQ(K35))*SQRT(SUMSQ(J36))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K35" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(L35),INDIRECT(K36)/(SQRT(SUMSQ(L35))*SQRT(SUMSQ(K36))))</f>
+        <v>#REF!</v>
+      </c>
       <c r="O35" t="s">
         <v>7</v>
       </c>
@@ -1377,7 +2394,19 @@
       <c r="U35" s="5"/>
       <c r="V35" s="6"/>
     </row>
-    <row r="36" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:22">
+      <c r="K36" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(L36),INDIRECT(K37)/(SQRT(SUMSQ(L36))*SQRT(SUMSQ(K37))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L36" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(M36),INDIRECT(L37)/(SQRT(SUMSQ(M36))*SQRT(SUMSQ(L37))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M36" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(N36),INDIRECT(M37)/(SQRT(SUMSQ(N36))*SQRT(SUMSQ(M37))))</f>
+        <v>#REF!</v>
+      </c>
       <c r="O36" t="s">
         <v>8</v>
       </c>
@@ -1391,7 +2420,15 @@
       <c r="U36" s="5"/>
       <c r="V36" s="6"/>
     </row>
-    <row r="37" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:22">
+      <c r="M37" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(N37),INDIRECT(M38)/(SQRT(SUMSQ(N37))*SQRT(SUMSQ(M38))))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N37" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(O37),INDIRECT(N38)/(SQRT(SUMSQ(O37))*SQRT(SUMSQ(N38))))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O37" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +2442,11 @@
       <c r="U37" s="5"/>
       <c r="V37" s="6"/>
     </row>
-    <row r="38" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:22">
+      <c r="N38" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(O38),INDIRECT(N39)/(SQRT(SUMSQ(O38))*SQRT(SUMSQ(N39))))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O38" t="s">
         <v>10</v>
       </c>
@@ -1419,7 +2460,7 @@
       <c r="U38" s="5"/>
       <c r="V38" s="6"/>
     </row>
-    <row r="39" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:22" ht="15.75" thickBot="1">
       <c r="C39" t="e">
         <f ca="1">SUMPRODUCT(INDIRECT(C40),INDIRECT(O39))/(SQRT(SUMSQ(C40))*SQRT(SUMSQ(O39)))</f>
         <v>#DIV/0!</v>
@@ -1428,6 +2469,10 @@
         <f ca="1">SUM(INDIRECT(O39))</f>
         <v>7</v>
       </c>
+      <c r="M39" t="e">
+        <f ca="1">SUMPRODUCT(INDIRECT(N39),INDIRECT(M40)/(SQRT(SUMSQ(N39))*SQRT(SUMSQ(M40))))</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="N39" t="e">
         <f ca="1">SUMPRODUCT(INDIRECT(O39),INDIRECT(N40)/(SQRT(SUMSQ(O39))*SQRT(SUMSQ(N40))))</f>
         <v>#DIV/0!</v>
@@ -1457,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:22">
       <c r="C40" t="s">
         <v>0</v>
       </c>
@@ -1509,5 +2554,454 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>7</v>
+      </c>
+      <c r="R9">
+        <f t="array" ref="R9:T11">MMULT(J9:L11,N9:P11)</f>
+        <v>21</v>
+      </c>
+      <c r="S9">
+        <v>45</v>
+      </c>
+      <c r="T9">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>8</v>
+      </c>
+      <c r="R10">
+        <v>21</v>
+      </c>
+      <c r="S10">
+        <v>48</v>
+      </c>
+      <c r="T10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>54</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>9</v>
+      </c>
+      <c r="R11">
+        <v>129</v>
+      </c>
+      <c r="S11">
+        <v>318</v>
+      </c>
+      <c r="T11">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="18" spans="10:23">
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>5</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f t="array" ref="U18:W22">MMULT(J18:M19,P18:R21)</f>
+        <v>7</v>
+      </c>
+      <c r="V18">
+        <v>6</v>
+      </c>
+      <c r="W18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="10:23">
+      <c r="J19">
+        <v>9</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>5</v>
+      </c>
+      <c r="U19">
+        <v>16</v>
+      </c>
+      <c r="V19">
+        <v>13</v>
+      </c>
+      <c r="W19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="10:23">
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>4</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="U20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V20" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W20" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="10:23">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="U21" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V21" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="10:23">
+      <c r="U22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W22" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="10:23">
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f t="array" ref="R25:T27">MMULT(J25:L27,N25:P27)</f>
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>4</v>
+      </c>
+      <c r="T25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="10:23">
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+      <c r="S26">
+        <v>2</v>
+      </c>
+      <c r="T26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="10:23">
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>2</v>
+      </c>
+      <c r="S27">
+        <v>5</v>
+      </c>
+      <c r="T27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="10:23">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>2</v>
+      </c>
+      <c r="R30">
+        <v>3</v>
+      </c>
+      <c r="S30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="10:23">
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>1</v>
+      </c>
+      <c r="S31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="10:23">
+      <c r="P32" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>22</v>
+      </c>
+      <c r="R32" t="s">
+        <v>23</v>
+      </c>
+      <c r="S32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="10:15">
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="10:15">
+      <c r="J34" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" t="s">
+        <v>26</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="10:15">
+      <c r="J35" t="s">
+        <v>21</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="10:15">
+      <c r="J36" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36">
+        <v>2</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>5</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="10:15">
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="10:15">
+      <c r="J38" t="s">
+        <v>24</v>
+      </c>
+      <c r="K38">
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>